<commit_message>
week 15, finals week fall 2016
</commit_message>
<xml_diff>
--- a/doc/comparison_matrix_qp.xlsx
+++ b/doc/comparison_matrix_qp.xlsx
@@ -14,6 +14,56 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v3.0" hidden="1">Sheet1!$A$10</definedName>
+    <definedName name="_xlchart.v3.1" hidden="1">Sheet1!$A$11</definedName>
+    <definedName name="_xlchart.v3.10" hidden="1">Sheet1!$A$9</definedName>
+    <definedName name="_xlchart.v3.11" hidden="1">Sheet1!$H$10:$N$10</definedName>
+    <definedName name="_xlchart.v3.12" hidden="1">Sheet1!$H$11:$N$11</definedName>
+    <definedName name="_xlchart.v3.13" hidden="1">Sheet1!$H$12:$N$12</definedName>
+    <definedName name="_xlchart.v3.14" hidden="1">Sheet1!$H$13:$N$13</definedName>
+    <definedName name="_xlchart.v3.15" hidden="1">Sheet1!$H$2:$N$2</definedName>
+    <definedName name="_xlchart.v3.16" hidden="1">Sheet1!$H$3:$N$3</definedName>
+    <definedName name="_xlchart.v3.17" hidden="1">Sheet1!$H$4:$N$4</definedName>
+    <definedName name="_xlchart.v3.18" hidden="1">Sheet1!$H$5:$N$5</definedName>
+    <definedName name="_xlchart.v3.19" hidden="1">Sheet1!$H$6:$N$6</definedName>
+    <definedName name="_xlchart.v3.2" hidden="1">Sheet1!$A$12</definedName>
+    <definedName name="_xlchart.v3.20" hidden="1">Sheet1!$H$7:$N$7</definedName>
+    <definedName name="_xlchart.v3.21" hidden="1">Sheet1!$H$8:$N$8</definedName>
+    <definedName name="_xlchart.v3.22" hidden="1">Sheet1!$H$9:$N$9</definedName>
+    <definedName name="_xlchart.v3.23" hidden="1">Sheet1!$H$9:$N$9</definedName>
+    <definedName name="_xlchart.v3.24" hidden="1">Sheet1!$A$10</definedName>
+    <definedName name="_xlchart.v3.25" hidden="1">Sheet1!$A$11</definedName>
+    <definedName name="_xlchart.v3.26" hidden="1">Sheet1!$A$12</definedName>
+    <definedName name="_xlchart.v3.27" hidden="1">Sheet1!$A$13</definedName>
+    <definedName name="_xlchart.v3.28" hidden="1">Sheet1!$A$3</definedName>
+    <definedName name="_xlchart.v3.29" hidden="1">Sheet1!$A$4</definedName>
+    <definedName name="_xlchart.v3.3" hidden="1">Sheet1!$A$13</definedName>
+    <definedName name="_xlchart.v3.30" hidden="1">Sheet1!$A$5</definedName>
+    <definedName name="_xlchart.v3.31" hidden="1">Sheet1!$A$6</definedName>
+    <definedName name="_xlchart.v3.32" hidden="1">Sheet1!$A$7</definedName>
+    <definedName name="_xlchart.v3.33" hidden="1">Sheet1!$A$8</definedName>
+    <definedName name="_xlchart.v3.34" hidden="1">Sheet1!$A$9</definedName>
+    <definedName name="_xlchart.v3.35" hidden="1">Sheet1!$H$10:$N$10</definedName>
+    <definedName name="_xlchart.v3.36" hidden="1">Sheet1!$H$11:$N$11</definedName>
+    <definedName name="_xlchart.v3.37" hidden="1">Sheet1!$H$12:$N$12</definedName>
+    <definedName name="_xlchart.v3.38" hidden="1">Sheet1!$H$13:$N$13</definedName>
+    <definedName name="_xlchart.v3.39" hidden="1">Sheet1!$H$2:$N$2</definedName>
+    <definedName name="_xlchart.v3.4" hidden="1">Sheet1!$A$3</definedName>
+    <definedName name="_xlchart.v3.40" hidden="1">Sheet1!$H$3:$N$3</definedName>
+    <definedName name="_xlchart.v3.41" hidden="1">Sheet1!$H$4:$N$4</definedName>
+    <definedName name="_xlchart.v3.42" hidden="1">Sheet1!$H$5:$N$5</definedName>
+    <definedName name="_xlchart.v3.43" hidden="1">Sheet1!$H$6:$N$6</definedName>
+    <definedName name="_xlchart.v3.44" hidden="1">Sheet1!$H$7:$N$7</definedName>
+    <definedName name="_xlchart.v3.45" hidden="1">Sheet1!$H$8:$N$8</definedName>
+    <definedName name="_xlchart.v3.46" hidden="1">Sheet1!$H$9:$N$9</definedName>
+    <definedName name="_xlchart.v3.47" hidden="1">Sheet1!$H$9:$N$9</definedName>
+    <definedName name="_xlchart.v3.5" hidden="1">Sheet1!$A$4</definedName>
+    <definedName name="_xlchart.v3.6" hidden="1">Sheet1!$A$5</definedName>
+    <definedName name="_xlchart.v3.7" hidden="1">Sheet1!$A$6</definedName>
+    <definedName name="_xlchart.v3.8" hidden="1">Sheet1!$A$7</definedName>
+    <definedName name="_xlchart.v3.9" hidden="1">Sheet1!$A$8</definedName>
+  </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -161,35 +211,10 @@
     <t>http://www.digikey.com/product-detail/en/luna-optoelectronics/PDB-C203/PDB-C203-ND/201823</t>
   </si>
   <si>
-    <r>
-      <t>Active Area (mm</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>) each</t>
-    </r>
-  </si>
-  <si>
     <t>Responsivity (A/W) @ Wavelength (nm)</t>
+  </si>
+  <si>
+    <t>Active Area (mm^2) each</t>
   </si>
 </sst>
 </file>
@@ -200,7 +225,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -227,15 +252,6 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <vertAlign val="superscript"/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -327,11 +343,33 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="22">
     <border>
       <left/>
       <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -351,8 +389,85 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color theme="1"/>
+      <left style="thick">
+        <color rgb="FF9F00FF"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color rgb="FF9F00FF"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF4B0082"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color rgb="FF4B0082"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF0000FF"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color rgb="FF0000FF"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF00FF00"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color rgb="FF00FF00"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFFFF00"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color rgb="FFFFFF00"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFF7F00"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color rgb="FFFF7F00"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFF0000"/>
       </left>
       <right/>
       <top style="thin">
@@ -379,8 +494,74 @@
         <color theme="1"/>
       </left>
       <right/>
-      <top style="medium">
+      <top style="thick">
+        <color rgb="FF9F00FF"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color theme="1"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color rgb="FF4B0082"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color rgb="FF0000FF"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color rgb="FF00FF00"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color rgb="FFFFFF00"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color rgb="FFFF7F00"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color rgb="FFFF0000"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -411,124 +592,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color theme="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color rgb="FF9F00FF"/>
-      </left>
-      <right/>
-      <top style="thick">
-        <color rgb="FF9F00FF"/>
-      </top>
-      <bottom style="thick">
-        <color rgb="FF9F00FF"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color rgb="FF4B0082"/>
-      </left>
-      <right/>
-      <top style="thick">
-        <color rgb="FF4B0082"/>
-      </top>
-      <bottom style="thick">
-        <color rgb="FF4B0082"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color rgb="FF0000FF"/>
-      </left>
-      <right/>
-      <top style="thick">
-        <color rgb="FF0000FF"/>
-      </top>
-      <bottom style="thick">
-        <color rgb="FF0000FF"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color rgb="FF00FF00"/>
-      </left>
-      <right/>
-      <top style="thick">
-        <color rgb="FF00FF00"/>
-      </top>
-      <bottom style="thick">
-        <color rgb="FF00FF00"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color rgb="FFFFFF00"/>
-      </left>
-      <right/>
-      <top style="thick">
-        <color rgb="FFFFFF00"/>
-      </top>
-      <bottom style="thick">
-        <color rgb="FFFFFF00"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color rgb="FFFF0000"/>
-      </left>
-      <right style="thick">
-        <color rgb="FFFF0000"/>
-      </right>
-      <top style="thick">
-        <color rgb="FFFF0000"/>
-      </top>
-      <bottom style="thick">
-        <color rgb="FFFF0000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color rgb="FFFF7F00"/>
-      </left>
-      <right/>
-      <top style="thick">
-        <color rgb="FFFF7F00"/>
-      </top>
-      <bottom style="thick">
-        <color rgb="FFFF7F00"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -556,49 +626,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -613,36 +647,90 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -819,19 +907,19 @@
                   <c:v>450</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>475</c:v>
+                  <c:v>480</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>575</c:v>
+                  <c:v>580</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>650</c:v>
+                  <c:v>640</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -948,19 +1036,19 @@
                   <c:v>450</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>475</c:v>
+                  <c:v>480</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>575</c:v>
+                  <c:v>580</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>650</c:v>
+                  <c:v>640</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -998,7 +1086,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-1FE0-40A9-A30C-617ADD5BF1BA}"/>
+              <c16:uniqueId val="{00000008-E726-4D14-B5C5-14D7DD96FDCF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1077,19 +1165,19 @@
                   <c:v>450</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>475</c:v>
+                  <c:v>480</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>575</c:v>
+                  <c:v>580</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>650</c:v>
+                  <c:v>640</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1127,7 +1215,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-1FE0-40A9-A30C-617ADD5BF1BA}"/>
+              <c16:uniqueId val="{00000009-E726-4D14-B5C5-14D7DD96FDCF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1206,19 +1294,19 @@
                   <c:v>450</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>475</c:v>
+                  <c:v>480</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>575</c:v>
+                  <c:v>580</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>650</c:v>
+                  <c:v>640</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1256,7 +1344,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-1FE0-40A9-A30C-617ADD5BF1BA}"/>
+              <c16:uniqueId val="{0000000A-E726-4D14-B5C5-14D7DD96FDCF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1335,19 +1423,19 @@
                   <c:v>450</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>475</c:v>
+                  <c:v>480</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>575</c:v>
+                  <c:v>580</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>650</c:v>
+                  <c:v>640</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1385,7 +1473,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-1FE0-40A9-A30C-617ADD5BF1BA}"/>
+              <c16:uniqueId val="{0000000B-E726-4D14-B5C5-14D7DD96FDCF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1464,19 +1552,19 @@
                   <c:v>450</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>475</c:v>
+                  <c:v>480</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>575</c:v>
+                  <c:v>580</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>650</c:v>
+                  <c:v>640</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1514,7 +1602,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-1FE0-40A9-A30C-617ADD5BF1BA}"/>
+              <c16:uniqueId val="{0000000C-E726-4D14-B5C5-14D7DD96FDCF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1600,19 +1688,19 @@
                   <c:v>450</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>475</c:v>
+                  <c:v>480</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>575</c:v>
+                  <c:v>580</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>650</c:v>
+                  <c:v>640</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1650,7 +1738,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-1FE0-40A9-A30C-617ADD5BF1BA}"/>
+              <c16:uniqueId val="{0000000D-E726-4D14-B5C5-14D7DD96FDCF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1736,19 +1824,19 @@
                   <c:v>450</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>475</c:v>
+                  <c:v>480</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>575</c:v>
+                  <c:v>580</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>650</c:v>
+                  <c:v>640</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1786,7 +1874,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000007-1FE0-40A9-A30C-617ADD5BF1BA}"/>
+              <c16:uniqueId val="{0000000E-E726-4D14-B5C5-14D7DD96FDCF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1872,19 +1960,19 @@
                   <c:v>450</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>475</c:v>
+                  <c:v>480</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>575</c:v>
+                  <c:v>580</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>650</c:v>
+                  <c:v>640</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1922,7 +2010,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000008-1FE0-40A9-A30C-617ADD5BF1BA}"/>
+              <c16:uniqueId val="{0000000F-E726-4D14-B5C5-14D7DD96FDCF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2008,19 +2096,19 @@
                   <c:v>450</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>475</c:v>
+                  <c:v>480</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>575</c:v>
+                  <c:v>580</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>650</c:v>
+                  <c:v>640</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2058,7 +2146,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000009-1FE0-40A9-A30C-617ADD5BF1BA}"/>
+              <c16:uniqueId val="{00000010-E726-4D14-B5C5-14D7DD96FDCF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2144,19 +2232,19 @@
                   <c:v>450</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>475</c:v>
+                  <c:v>480</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>575</c:v>
+                  <c:v>580</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>650</c:v>
+                  <c:v>640</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2194,7 +2282,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000A-1FE0-40A9-A30C-617ADD5BF1BA}"/>
+              <c16:uniqueId val="{00000011-E726-4D14-B5C5-14D7DD96FDCF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2213,8 +2301,7 @@
         <c:axId val="1964365583"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="650"/>
-          <c:min val="400"/>
+          <c:min val="350"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -2287,13 +2374,14 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx2">
                 <a:lumMod val="40000"/>
                 <a:lumOff val="60000"/>
               </a:schemeClr>
             </a:solidFill>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -3358,7 +3446,7 @@
   <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S17" sqref="S17"/>
+      <selection activeCell="V17" sqref="V17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -3366,13 +3454,13 @@
     <col min="1" max="1" width="15" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.4609375" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.765625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="10.765625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="10.53515625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10.4609375" style="5" customWidth="1"/>
+    <col min="4" max="4" width="11.3828125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="9.53515625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="11.69140625" style="5" customWidth="1"/>
     <col min="7" max="7" width="17.3828125" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="14" width="5.69140625" style="5" customWidth="1"/>
+    <col min="8" max="14" width="5.921875" style="5" customWidth="1"/>
     <col min="15" max="15" width="17.765625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="23.84375" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.921875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="16.3" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
@@ -3383,597 +3471,597 @@
       <c r="E1" s="8"/>
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
-      <c r="H1" s="44" t="s">
-        <v>46</v>
-      </c>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
-      <c r="N1" s="44"/>
+      <c r="H1" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
       <c r="O1" s="9"/>
       <c r="P1" s="10"/>
     </row>
     <row r="2" spans="1:16" s="9" customFormat="1" ht="29.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="G2" s="14" t="s">
+      <c r="F2" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="36">
+      <c r="H2" s="28">
         <v>400</v>
       </c>
-      <c r="I2" s="37">
+      <c r="I2" s="29">
         <v>450</v>
       </c>
-      <c r="J2" s="38">
-        <v>475</v>
-      </c>
-      <c r="K2" s="39">
+      <c r="J2" s="30">
+        <v>480</v>
+      </c>
+      <c r="K2" s="31">
         <v>500</v>
       </c>
-      <c r="L2" s="40">
-        <v>575</v>
-      </c>
-      <c r="M2" s="41">
+      <c r="L2" s="32">
+        <v>580</v>
+      </c>
+      <c r="M2" s="33">
         <v>600</v>
       </c>
-      <c r="N2" s="43">
-        <v>650</v>
-      </c>
-      <c r="O2" s="42" t="s">
+      <c r="N2" s="34">
+        <v>640</v>
+      </c>
+      <c r="O2" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="P2" s="15" t="s">
+      <c r="P2" s="36" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="29.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="17">
+      <c r="B3" s="15">
         <v>5.98</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="18">
+      <c r="D3" s="16">
         <v>890</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="18">
+      <c r="F3" s="16">
         <v>0.75</v>
       </c>
-      <c r="G3" s="19" t="s">
+      <c r="G3" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="35">
+      <c r="H3" s="37">
         <v>0.14000000000000001</v>
       </c>
-      <c r="I3" s="35">
+      <c r="I3" s="38">
         <v>0.19</v>
       </c>
-      <c r="J3" s="35">
+      <c r="J3" s="39">
         <v>0.21</v>
       </c>
-      <c r="K3" s="35">
+      <c r="K3" s="40">
         <v>0.22</v>
       </c>
-      <c r="L3" s="35">
+      <c r="L3" s="41">
         <v>0.31</v>
       </c>
-      <c r="M3" s="35">
+      <c r="M3" s="42">
         <v>0.34499999999999997</v>
       </c>
-      <c r="N3" s="35">
+      <c r="N3" s="43">
         <v>0.4</v>
       </c>
-      <c r="O3" s="16"/>
-      <c r="P3" s="20" t="s">
+      <c r="O3" s="14"/>
+      <c r="P3" s="44" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="22">
+      <c r="B4" s="19">
         <v>72.38</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="23">
+      <c r="D4" s="20">
         <v>660</v>
       </c>
-      <c r="E4" s="22" t="s">
+      <c r="E4" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="23">
+      <c r="F4" s="20">
         <v>1.145</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="G4" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="H4" s="23">
+      <c r="H4" s="20">
         <v>0.14000000000000001</v>
       </c>
-      <c r="I4" s="23">
+      <c r="I4" s="20">
         <v>0.19</v>
       </c>
-      <c r="J4" s="23">
+      <c r="J4" s="20">
         <v>0.21</v>
       </c>
-      <c r="K4" s="23">
+      <c r="K4" s="20">
         <v>0.22</v>
       </c>
-      <c r="L4" s="23">
+      <c r="L4" s="20">
         <v>0.31</v>
       </c>
-      <c r="M4" s="23">
+      <c r="M4" s="20">
         <v>0.35</v>
       </c>
-      <c r="N4" s="23">
+      <c r="N4" s="20">
         <v>0.4</v>
       </c>
-      <c r="O4" s="21"/>
-      <c r="P4" s="25" t="s">
+      <c r="O4" s="18"/>
+      <c r="P4" s="45" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="27">
+      <c r="B5" s="23">
         <v>107.81</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="28">
+      <c r="D5" s="24">
         <v>660</v>
       </c>
-      <c r="E5" s="27" t="s">
+      <c r="E5" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="28">
+      <c r="F5" s="24">
         <v>2.25</v>
       </c>
-      <c r="G5" s="29" t="s">
+      <c r="G5" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="H5" s="28">
+      <c r="H5" s="24">
         <v>0.14000000000000001</v>
       </c>
-      <c r="I5" s="28">
+      <c r="I5" s="24">
         <v>0.19</v>
       </c>
-      <c r="J5" s="28">
+      <c r="J5" s="24">
         <v>0.21</v>
       </c>
-      <c r="K5" s="28">
+      <c r="K5" s="24">
         <v>0.23</v>
       </c>
-      <c r="L5" s="28">
+      <c r="L5" s="24">
         <v>0.32</v>
       </c>
-      <c r="M5" s="28">
+      <c r="M5" s="24">
         <v>0.35</v>
       </c>
-      <c r="N5" s="28">
+      <c r="N5" s="24">
         <v>0.4</v>
       </c>
-      <c r="O5" s="26"/>
-      <c r="P5" s="30" t="s">
+      <c r="O5" s="22"/>
+      <c r="P5" s="46" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="22">
+      <c r="B6" s="19">
         <v>100.05</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="23">
+      <c r="D6" s="20">
         <v>660</v>
       </c>
-      <c r="E6" s="22" t="s">
+      <c r="E6" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="23">
+      <c r="F6" s="20">
         <v>2.355</v>
       </c>
-      <c r="G6" s="24" t="s">
+      <c r="G6" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="H6" s="23">
+      <c r="H6" s="20">
         <v>0.14000000000000001</v>
       </c>
-      <c r="I6" s="23">
+      <c r="I6" s="20">
         <v>0.18</v>
       </c>
-      <c r="J6" s="23">
+      <c r="J6" s="20">
         <v>0.20499999999999999</v>
       </c>
-      <c r="K6" s="23">
+      <c r="K6" s="20">
         <v>0.23</v>
       </c>
-      <c r="L6" s="23">
+      <c r="L6" s="20">
         <v>0.315</v>
       </c>
-      <c r="M6" s="23">
+      <c r="M6" s="20">
         <v>0.35</v>
       </c>
-      <c r="N6" s="23">
+      <c r="N6" s="20">
         <v>0.4</v>
       </c>
-      <c r="O6" s="21"/>
-      <c r="P6" s="25" t="s">
+      <c r="O6" s="18"/>
+      <c r="P6" s="45" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="27">
+      <c r="B7" s="23">
         <v>93.02</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="28">
+      <c r="D7" s="24">
         <v>660</v>
       </c>
-      <c r="E7" s="27" t="s">
+      <c r="E7" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="28">
+      <c r="F7" s="24">
         <v>5.2220000000000004</v>
       </c>
-      <c r="G7" s="29" t="s">
+      <c r="G7" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="H7" s="28">
+      <c r="H7" s="24">
         <v>0.14000000000000001</v>
       </c>
-      <c r="I7" s="28">
+      <c r="I7" s="24">
         <v>0.18</v>
       </c>
-      <c r="J7" s="28">
+      <c r="J7" s="24">
         <v>0.21</v>
       </c>
-      <c r="K7" s="28">
+      <c r="K7" s="24">
         <v>0.22</v>
       </c>
-      <c r="L7" s="28">
+      <c r="L7" s="24">
         <v>0.32</v>
       </c>
-      <c r="M7" s="28">
+      <c r="M7" s="24">
         <v>0.34499999999999997</v>
       </c>
-      <c r="N7" s="28">
+      <c r="N7" s="24">
         <v>0.4</v>
       </c>
-      <c r="O7" s="26" t="s">
+      <c r="O7" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="P7" s="30" t="s">
+      <c r="P7" s="46" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="22">
+      <c r="B8" s="19">
         <v>60.36</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="23">
+      <c r="D8" s="20">
         <v>950</v>
       </c>
-      <c r="E8" s="22" t="s">
+      <c r="E8" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="23">
+      <c r="F8" s="20">
         <v>1.69</v>
       </c>
-      <c r="G8" s="24" t="s">
+      <c r="G8" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="H8" s="23">
+      <c r="H8" s="20">
         <v>0.12</v>
       </c>
-      <c r="I8" s="23">
+      <c r="I8" s="20">
         <v>0.2</v>
       </c>
-      <c r="J8" s="23">
+      <c r="J8" s="20">
         <v>0.24</v>
       </c>
-      <c r="K8" s="23">
+      <c r="K8" s="20">
         <v>0.28000000000000003</v>
       </c>
-      <c r="L8" s="23">
+      <c r="L8" s="20">
         <v>0.36</v>
       </c>
-      <c r="M8" s="23">
+      <c r="M8" s="20">
         <v>0.4</v>
       </c>
-      <c r="N8" s="23">
+      <c r="N8" s="20">
         <v>0.45</v>
       </c>
-      <c r="O8" s="21"/>
-      <c r="P8" s="25" t="s">
+      <c r="O8" s="18"/>
+      <c r="P8" s="45" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="27">
+      <c r="B9" s="23">
         <v>40</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="28">
+      <c r="D9" s="24">
         <v>900</v>
       </c>
-      <c r="E9" s="27" t="s">
+      <c r="E9" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="28">
+      <c r="F9" s="24">
         <v>0.25</v>
       </c>
-      <c r="G9" s="29" t="s">
+      <c r="G9" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="H9" s="28">
+      <c r="H9" s="24">
         <v>0.18</v>
       </c>
-      <c r="I9" s="28">
+      <c r="I9" s="24">
         <v>0.17499999999999999</v>
       </c>
-      <c r="J9" s="28">
+      <c r="J9" s="24">
         <v>0.2</v>
       </c>
-      <c r="K9" s="28">
+      <c r="K9" s="24">
         <v>0.23</v>
       </c>
-      <c r="L9" s="28">
+      <c r="L9" s="24">
         <v>0.32500000000000001</v>
       </c>
-      <c r="M9" s="28">
+      <c r="M9" s="24">
         <v>0.38</v>
       </c>
-      <c r="N9" s="28">
+      <c r="N9" s="24">
         <v>0.42</v>
       </c>
-      <c r="O9" s="26"/>
-      <c r="P9" s="30" t="s">
+      <c r="O9" s="22"/>
+      <c r="P9" s="46" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="22">
+      <c r="B10" s="19">
         <v>44.54</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="C10" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="23">
+      <c r="D10" s="20">
         <v>633</v>
       </c>
-      <c r="E10" s="22" t="s">
+      <c r="E10" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="23">
+      <c r="F10" s="20">
         <v>1.44</v>
       </c>
-      <c r="G10" s="24" t="s">
+      <c r="G10" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="H10" s="23">
+      <c r="H10" s="20">
         <v>0.1</v>
       </c>
-      <c r="I10" s="23">
+      <c r="I10" s="20">
         <v>0.15</v>
       </c>
-      <c r="J10" s="23">
+      <c r="J10" s="20">
         <v>0.18</v>
       </c>
-      <c r="K10" s="23">
+      <c r="K10" s="20">
         <v>0.215</v>
       </c>
-      <c r="L10" s="23">
+      <c r="L10" s="20">
         <v>0.35</v>
       </c>
-      <c r="M10" s="23">
+      <c r="M10" s="20">
         <v>0.39</v>
       </c>
-      <c r="N10" s="23">
+      <c r="N10" s="20">
         <v>0.45</v>
       </c>
-      <c r="O10" s="21"/>
-      <c r="P10" s="25" t="s">
+      <c r="O10" s="18"/>
+      <c r="P10" s="45" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="26" t="s">
+      <c r="A11" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="27">
+      <c r="B11" s="23">
         <v>52.25</v>
       </c>
-      <c r="C11" s="27" t="s">
+      <c r="C11" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="28">
+      <c r="D11" s="24">
         <v>900</v>
       </c>
-      <c r="E11" s="27" t="s">
+      <c r="E11" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="28">
+      <c r="F11" s="24">
         <v>2.4500000000000002</v>
       </c>
-      <c r="G11" s="29" t="s">
+      <c r="G11" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="H11" s="28">
+      <c r="H11" s="24">
         <v>0.09</v>
       </c>
-      <c r="I11" s="28">
+      <c r="I11" s="24">
         <v>0.16500000000000001</v>
       </c>
-      <c r="J11" s="28">
+      <c r="J11" s="24">
         <v>0.2</v>
       </c>
-      <c r="K11" s="28">
+      <c r="K11" s="24">
         <v>0.22500000000000001</v>
       </c>
-      <c r="L11" s="28">
+      <c r="L11" s="24">
         <v>0.33</v>
       </c>
-      <c r="M11" s="28">
+      <c r="M11" s="24">
         <v>0.38</v>
       </c>
-      <c r="N11" s="28">
+      <c r="N11" s="24">
         <v>0.42</v>
       </c>
-      <c r="O11" s="26"/>
-      <c r="P11" s="30" t="s">
+      <c r="O11" s="22"/>
+      <c r="P11" s="46" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="22">
+      <c r="B12" s="19">
         <v>142.37</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="C12" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="23">
+      <c r="D12" s="20">
         <v>850</v>
       </c>
-      <c r="E12" s="22" t="s">
+      <c r="E12" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="F12" s="23">
+      <c r="F12" s="20">
         <v>12</v>
       </c>
-      <c r="G12" s="24" t="s">
+      <c r="G12" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="H12" s="23">
+      <c r="H12" s="20">
         <v>0.09</v>
       </c>
-      <c r="I12" s="23">
+      <c r="I12" s="20">
         <v>0.16</v>
       </c>
-      <c r="J12" s="23">
+      <c r="J12" s="20">
         <v>0.2</v>
       </c>
-      <c r="K12" s="23">
+      <c r="K12" s="20">
         <v>0.23</v>
       </c>
-      <c r="L12" s="23">
+      <c r="L12" s="20">
         <v>0.33</v>
       </c>
-      <c r="M12" s="23">
+      <c r="M12" s="20">
         <v>0.38</v>
       </c>
-      <c r="N12" s="23">
+      <c r="N12" s="20">
         <v>0.42</v>
       </c>
-      <c r="O12" s="21"/>
-      <c r="P12" s="25" t="s">
+      <c r="O12" s="18"/>
+      <c r="P12" s="45" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="32">
+      <c r="B13" s="48">
         <v>156.44</v>
       </c>
-      <c r="C13" s="32" t="s">
+      <c r="C13" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="33">
+      <c r="D13" s="49">
         <v>633</v>
       </c>
-      <c r="E13" s="32" t="s">
+      <c r="E13" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="F13" s="33">
+      <c r="F13" s="49">
         <v>24.35</v>
       </c>
-      <c r="G13" s="34" t="s">
+      <c r="G13" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="H13" s="33">
+      <c r="H13" s="49">
         <v>0.09</v>
       </c>
-      <c r="I13" s="33">
+      <c r="I13" s="49">
         <v>0.18</v>
       </c>
-      <c r="J13" s="33">
+      <c r="J13" s="49">
         <v>0.20499999999999999</v>
       </c>
-      <c r="K13" s="33">
+      <c r="K13" s="49">
         <v>0.22500000000000001</v>
       </c>
-      <c r="L13" s="33">
+      <c r="L13" s="49">
         <v>0.35</v>
       </c>
-      <c r="M13" s="33">
+      <c r="M13" s="49">
         <v>0.38</v>
       </c>
-      <c r="N13" s="33">
+      <c r="N13" s="49">
         <v>0.42</v>
       </c>
-      <c r="O13" s="31" t="s">
+      <c r="O13" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="P13" s="11" t="s">
+      <c r="P13" s="27" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>